<commit_message>
MOSIP-30269 Added preferredLang for all languages (#278)
Signed-off-by: kameshsr <kameshsr1338@gmail.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/dynamic_field.xlsx
+++ b/mosip_master/xlsx/dynamic_field.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{699A50B2-0AA9-429B-BD65-38D53DE3E703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D803672-6D09-4806-93DA-AAA3B9FB13F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$205</definedName>
     <definedName name="_FilterDatabase_0" localSheetId="0">Sheet1!$A$1:$I$103</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -29,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1689" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1905" uniqueCount="253">
   <si>
     <t>id</t>
   </si>
@@ -1479,6 +1488,15 @@
   </si>
   <si>
     <t>{"value":"Española","code":"spa"}</t>
+  </si>
+  <si>
+    <t>{"value":"ಕನ್ನಡ","code":"kan"}</t>
+  </si>
+  <si>
+    <t>{"value":"हिंदी","code":"hin"}</t>
+  </si>
+  <si>
+    <t>{"value":"தமிழ்","code":"tam"}</t>
   </si>
 </sst>
 </file>
@@ -1859,10 +1877,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I212"/>
+  <dimension ref="A1:I239"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A209" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E214" sqref="E214"/>
+    <sheetView tabSelected="1" topLeftCell="A233" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C240" sqref="C240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8002,6 +8020,816 @@
         <v>16</v>
       </c>
     </row>
+    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A213" s="2">
+        <f>SUM(A212,1)</f>
+        <v>10212</v>
+      </c>
+      <c r="B213" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C213" t="s">
+        <v>57</v>
+      </c>
+      <c r="D213" t="s">
+        <v>11</v>
+      </c>
+      <c r="E213" t="s">
+        <v>249</v>
+      </c>
+      <c r="F213" t="s">
+        <v>13</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H213" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I213" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="214" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A214" s="2">
+        <f t="shared" ref="A214:A239" si="0">SUM(A213,1)</f>
+        <v>10213</v>
+      </c>
+      <c r="B214" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C214" t="s">
+        <v>57</v>
+      </c>
+      <c r="D214" t="s">
+        <v>11</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F214" t="s">
+        <v>13</v>
+      </c>
+      <c r="G214" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H214" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I214" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="215" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A215" s="2">
+        <f t="shared" si="0"/>
+        <v>10214</v>
+      </c>
+      <c r="B215" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C215" t="s">
+        <v>57</v>
+      </c>
+      <c r="D215" t="s">
+        <v>11</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F215" t="s">
+        <v>13</v>
+      </c>
+      <c r="G215" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H215" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I215" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="216" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A216" s="2">
+        <f t="shared" si="0"/>
+        <v>10215</v>
+      </c>
+      <c r="B216" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C216" t="s">
+        <v>57</v>
+      </c>
+      <c r="D216" t="s">
+        <v>11</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F216" t="s">
+        <v>13</v>
+      </c>
+      <c r="G216" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H216" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I216" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A217" s="2">
+        <f t="shared" si="0"/>
+        <v>10216</v>
+      </c>
+      <c r="B217" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C217" t="s">
+        <v>60</v>
+      </c>
+      <c r="D217" t="s">
+        <v>11</v>
+      </c>
+      <c r="E217" t="s">
+        <v>249</v>
+      </c>
+      <c r="F217" t="s">
+        <v>61</v>
+      </c>
+      <c r="G217" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H217" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I217" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="218" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A218" s="2">
+        <f t="shared" si="0"/>
+        <v>10217</v>
+      </c>
+      <c r="B218" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C218" t="s">
+        <v>60</v>
+      </c>
+      <c r="D218" t="s">
+        <v>11</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F218" t="s">
+        <v>61</v>
+      </c>
+      <c r="G218" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H218" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I218" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="219" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A219" s="2">
+        <f t="shared" si="0"/>
+        <v>10218</v>
+      </c>
+      <c r="B219" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C219" t="s">
+        <v>60</v>
+      </c>
+      <c r="D219" t="s">
+        <v>11</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F219" t="s">
+        <v>61</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H219" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I219" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="220" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A220" s="2">
+        <f t="shared" si="0"/>
+        <v>10219</v>
+      </c>
+      <c r="B220" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C220" t="s">
+        <v>60</v>
+      </c>
+      <c r="D220" t="s">
+        <v>11</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F220" t="s">
+        <v>61</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H220" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I220" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A221" s="2">
+        <f t="shared" si="0"/>
+        <v>10220</v>
+      </c>
+      <c r="B221" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C221" t="s">
+        <v>121</v>
+      </c>
+      <c r="D221" t="s">
+        <v>11</v>
+      </c>
+      <c r="E221" t="s">
+        <v>249</v>
+      </c>
+      <c r="F221" t="s">
+        <v>89</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H221" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I221" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="222" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A222" s="2">
+        <f t="shared" si="0"/>
+        <v>10221</v>
+      </c>
+      <c r="B222" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C222" t="s">
+        <v>121</v>
+      </c>
+      <c r="D222" t="s">
+        <v>11</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F222" t="s">
+        <v>89</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H222" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I222" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A223" s="2">
+        <f t="shared" si="0"/>
+        <v>10222</v>
+      </c>
+      <c r="B223" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C223" t="s">
+        <v>121</v>
+      </c>
+      <c r="D223" t="s">
+        <v>11</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F223" t="s">
+        <v>89</v>
+      </c>
+      <c r="G223" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H223" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I223" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="224" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A224" s="2">
+        <f t="shared" si="0"/>
+        <v>10223</v>
+      </c>
+      <c r="B224" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C224" t="s">
+        <v>121</v>
+      </c>
+      <c r="D224" t="s">
+        <v>11</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F224" t="s">
+        <v>89</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H224" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I224" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="225" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A225" s="2">
+        <f t="shared" si="0"/>
+        <v>10224</v>
+      </c>
+      <c r="B225" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C225" t="s">
+        <v>248</v>
+      </c>
+      <c r="D225" t="s">
+        <v>11</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F225" t="s">
+        <v>243</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H225" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I225" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="226" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A226" s="2">
+        <f t="shared" si="0"/>
+        <v>10225</v>
+      </c>
+      <c r="B226" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C226" t="s">
+        <v>248</v>
+      </c>
+      <c r="D226" t="s">
+        <v>11</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F226" t="s">
+        <v>243</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H226" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I226" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="227" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A227" s="2">
+        <f t="shared" si="0"/>
+        <v>10226</v>
+      </c>
+      <c r="B227" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C227" t="s">
+        <v>248</v>
+      </c>
+      <c r="D227" t="s">
+        <v>11</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F227" t="s">
+        <v>243</v>
+      </c>
+      <c r="G227" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H227" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I227" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A228" s="2">
+        <f t="shared" si="0"/>
+        <v>10227</v>
+      </c>
+      <c r="B228" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C228" t="s">
+        <v>162</v>
+      </c>
+      <c r="D228" t="s">
+        <v>11</v>
+      </c>
+      <c r="E228" t="s">
+        <v>249</v>
+      </c>
+      <c r="F228" t="s">
+        <v>126</v>
+      </c>
+      <c r="G228" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H228" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I228" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="229" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A229" s="2">
+        <f t="shared" si="0"/>
+        <v>10228</v>
+      </c>
+      <c r="B229" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C229" t="s">
+        <v>162</v>
+      </c>
+      <c r="D229" t="s">
+        <v>11</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F229" t="s">
+        <v>126</v>
+      </c>
+      <c r="G229" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H229" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I229" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="230" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A230" s="2">
+        <f t="shared" si="0"/>
+        <v>10229</v>
+      </c>
+      <c r="B230" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C230" t="s">
+        <v>162</v>
+      </c>
+      <c r="D230" t="s">
+        <v>11</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F230" t="s">
+        <v>126</v>
+      </c>
+      <c r="G230" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H230" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I230" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A231" s="2">
+        <f t="shared" si="0"/>
+        <v>10230</v>
+      </c>
+      <c r="B231" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C231" t="s">
+        <v>162</v>
+      </c>
+      <c r="D231" t="s">
+        <v>11</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F231" t="s">
+        <v>126</v>
+      </c>
+      <c r="G231" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H231" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I231" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A232" s="2">
+        <f t="shared" si="0"/>
+        <v>10231</v>
+      </c>
+      <c r="B232" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C232" t="s">
+        <v>202</v>
+      </c>
+      <c r="D232" t="s">
+        <v>11</v>
+      </c>
+      <c r="E232" t="s">
+        <v>249</v>
+      </c>
+      <c r="F232" t="s">
+        <v>166</v>
+      </c>
+      <c r="G232" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H232" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I232" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="233" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A233" s="2">
+        <f t="shared" si="0"/>
+        <v>10232</v>
+      </c>
+      <c r="B233" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C233" t="s">
+        <v>202</v>
+      </c>
+      <c r="D233" t="s">
+        <v>11</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F233" t="s">
+        <v>166</v>
+      </c>
+      <c r="G233" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H233" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I233" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="234" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A234" s="2">
+        <f t="shared" si="0"/>
+        <v>10233</v>
+      </c>
+      <c r="B234" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C234" t="s">
+        <v>202</v>
+      </c>
+      <c r="D234" t="s">
+        <v>11</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F234" t="s">
+        <v>166</v>
+      </c>
+      <c r="G234" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H234" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I234" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="235" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A235" s="2">
+        <f t="shared" si="0"/>
+        <v>10234</v>
+      </c>
+      <c r="B235" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C235" t="s">
+        <v>202</v>
+      </c>
+      <c r="D235" t="s">
+        <v>11</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F235" t="s">
+        <v>166</v>
+      </c>
+      <c r="G235" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H235" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I235" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A236" s="2">
+        <f t="shared" si="0"/>
+        <v>10235</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C236" t="s">
+        <v>242</v>
+      </c>
+      <c r="D236" t="s">
+        <v>11</v>
+      </c>
+      <c r="E236" t="s">
+        <v>249</v>
+      </c>
+      <c r="F236" t="s">
+        <v>205</v>
+      </c>
+      <c r="G236" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H236" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I236" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="237" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A237" s="2">
+        <f t="shared" si="0"/>
+        <v>10236</v>
+      </c>
+      <c r="B237" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C237" t="s">
+        <v>242</v>
+      </c>
+      <c r="D237" t="s">
+        <v>11</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="F237" t="s">
+        <v>205</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H237" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I237" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="238" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A238" s="2">
+        <f t="shared" si="0"/>
+        <v>10237</v>
+      </c>
+      <c r="B238" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C238" t="s">
+        <v>242</v>
+      </c>
+      <c r="D238" t="s">
+        <v>11</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F238" t="s">
+        <v>205</v>
+      </c>
+      <c r="G238" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H238" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I238" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A239" s="2">
+        <f t="shared" si="0"/>
+        <v>10238</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C239" t="s">
+        <v>242</v>
+      </c>
+      <c r="D239" t="s">
+        <v>11</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F239" t="s">
+        <v>205</v>
+      </c>
+      <c r="G239" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H239" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I239" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I205" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>